<commit_message>
import_user add gender support
</commit_message>
<xml_diff>
--- a/spec/data/user_import_test_files/user.xlsx
+++ b/spec/data/user_import_test_files/user.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="123820"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9230"/>
   </bookViews>
   <sheets>
     <sheet name="_e7_94_a8_e6_88_b7_e7_ae_a1_e7_" sheetId="1" r:id="rId1"/>
@@ -34,22 +34,26 @@
     <t>hello1</t>
   </si>
   <si>
-    <t>hi3@gmail.com</t>
-  </si>
-  <si>
-    <t>hi1@gmail.com</t>
-  </si>
-  <si>
     <t>hello2</t>
   </si>
   <si>
     <t>hello3</t>
   </si>
   <si>
-    <t>hi2@gmail.com</t>
-  </si>
-  <si>
-    <t>邮箱</t>
+    <t>性别</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>男</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>女</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>男</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -62,7 +66,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -82,12 +86,6 @@
     <font>
       <sz val="12"/>
       <name val="SimSun"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="12"/>
-      <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
@@ -141,7 +139,7 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0"/>
@@ -159,11 +157,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -465,14 +463,14 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D65536"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.125" customWidth="1"/>
+    <col min="1" max="1" width="19.08203125" customWidth="1"/>
     <col min="2" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="33.375" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -483,7 +481,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -493,8 +491,8 @@
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
+      <c r="C2" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -502,9 +500,9 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -513,21 +511,16 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-  </hyperlinks>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>

</xml_diff>